<commit_message>
Changed R & S to Y & S for twizzlers candies.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -464,7 +464,7 @@
     <col min="11" max="11" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:50">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,8 +493,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10"/>
-    <row r="3" spans="1:10">
+    <row r="2" spans="1:50"/>
+    <row r="3" spans="1:50">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -505,7 +505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:50">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -516,7 +516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:50">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -527,7 +527,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:50">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -538,12 +538,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10"/>
-    <row r="8" spans="1:10"/>
-    <row r="9" spans="1:10"/>
-    <row r="10" spans="1:10"/>
-    <row r="11" spans="1:10"/>
-    <row r="12" spans="1:10"/>
+    <row r="7" spans="1:50"/>
+    <row r="8" spans="1:50"/>
+    <row r="9" spans="1:50"/>
+    <row r="10" spans="1:50"/>
+    <row r="11" spans="1:50"/>
+    <row r="12" spans="1:50"/>
+    <row r="13" spans="1:50"/>
+    <row r="14" spans="1:50"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>